<commit_message>
Fix: Enhance LB domain transformation for horizontal data
</commit_message>
<xml_diff>
--- a/sdtm_workspace/mapping_specs/dm_mapping_specification.xlsx
+++ b/sdtm_workspace/mapping_specs/dm_mapping_specification.xlsx
@@ -519,7 +519,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Study identifier from source STUDY column (MAXIS-08)</t>
+          <t>Study identifier from STUDY source column (MAXIS-08)</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Parse PT to extract site and subject, concatenate with STUDY</t>
+          <t>Concatenate STUDY, SITEID, and SUBJID with hyphens</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -601,7 +601,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Unique subject identifier derived from STUDY + parsed PT field (format: MAXIS-08-01-01)</t>
+          <t>Unique subject identifier. PT contains 'SITEID-SUBJID' format. Example: MAXIS-08-01-01</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Extract subject number from PT after hyphen</t>
+          <t>Extract subject ID from PT field</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -644,7 +644,7 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Subject identifier extracted from PT field (second component)</t>
+          <t>Subject identifier within the study, extracted from second part of PT</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Extract site number from PT before hyphen</t>
+          <t>Extract site ID from PT field</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -687,7 +687,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Site identifier extracted from PT field (first component)</t>
+          <t>Study site identifier, extracted from first part of PT</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Direct mapping to CDISC SEX codelist</t>
+          <t>Direct mapping - already in correct format</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -729,29 +729,29 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>SEX (M=Male, F=Female, U=Unknown)</t>
+          <t>SEX</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Map source GENDER (M/F) directly to SEX using CDISC controlled terminology</t>
+          <t>Sex of subject. Source GENDER contains 'M' or 'F' which aligns with CDISC SEX codelist (M, F, U, UNDIFFERENTIATED)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ARMCD</t>
+          <t>RACE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Planned Arm Code</t>
+          <t>Race</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -767,25 +767,29 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>MAP</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>RACE</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Required variable - needs to be populated from separate randomization/treatment assignment dataset</t>
+          <t>Race mapping requires careful handling. HISPANIC in source should be considered for ETHNIC variable. Map to appropriate CDISC RACE terms</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ARM</t>
+          <t>ETHNIC</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Description of Planned Arm</t>
+          <t>Ethnicity</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -800,19 +804,27 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>RCE</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Map source RCE values to CDISC ETHNIC codelist</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
+          <t>MAP</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>ETHNIC</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Required variable - description of planned arm, needs to be populated from separate dataset</t>
+          <t>Ethnicity derived from RCE. HISPANIC values should populate ETHNIC variable per CDISC standards</t>
         </is>
       </c>
     </row>
@@ -844,7 +856,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Extract country code from INVSITE and map to ISO 3166 3-character code</t>
+          <t>Extract country code and map to ISO 3166 alpha-3</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -854,34 +866,34 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>ISO 3166 (3-character country codes)</t>
+          <t>ISO 3166</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Country derived from INVSITE field, requires mapping to ISO 3166 standard (e.g., USA, GBR, CAN)</t>
+          <t>Country code derived from INVSITE. C008 likely represents a country identifier that needs mapping to 3-character ISO code</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RFSTDTC</t>
+          <t>ARMCD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Subject Reference Start Date/Time</t>
+          <t>Planned Arm Code</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Req</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -892,25 +904,25 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Required - Subject reference start date, typically date of first dose or first visit, needs external data</t>
+          <t>Planned arm code - requires integration with randomization data or treatment assignment module</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RFENDTC</t>
+          <t>ARM</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Subject Reference End Date/Time</t>
+          <t>Description of Planned Arm</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -920,7 +932,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Req</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -931,30 +943,30 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Required - Subject reference end date, typically date of last contact, needs external data</t>
+          <t>Description of planned arm - requires integration with randomization data or treatment assignment module</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RFXSTDTC</t>
+          <t>ACTARMCD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Date/Time of First Study Treatment</t>
+          <t>Actual Arm Code</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -970,25 +982,25 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Expected variable - date/time of first study treatment, derive from EX domain</t>
+          <t>Actual arm code - derived from treatment exposure records, not available in demographics source</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RFXENDTC</t>
+          <t>ACTARM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Date/Time of Last Study Treatment</t>
+          <t>Description of Actual Arm</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1009,25 +1021,25 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Expected variable - date/time of last study treatment, derive from EX domain</t>
+          <t>Description of actual arm - derived from treatment exposure records</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RFICDTC</t>
+          <t>BRTHDTC</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Date/Time of Informed Consent</t>
+          <t>Date/Time of Birth</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1037,36 +1049,40 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
+          <t>DOB</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Convert YYYYMMDD integer to ISO 8601 format YYYY-MM-DD</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Expected variable - date/time of informed consent, needs to be sourced from enrollment records</t>
+          <t>Date of birth conversion. Source is integer YYYYMMDD format, convert to ISO 8601 string</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RFPENDTC</t>
+          <t>AGE</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Date/Time of End of Participation</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1076,7 +1092,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1087,25 +1103,25 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Expected variable - date/time of end of participation, derive from DS domain</t>
+          <t>Age in years at reference start date. Requires RFSTDTC to be determined from first study activity</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DTHDTC</t>
+          <t>AGEU</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Date/Time of Death</t>
+          <t>Age Units</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1115,7 +1131,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1129,22 +1145,26 @@
           <t>DERIVE</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>AGEU</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Expected variable - date/time of death if applicable, derive from DS or AE domains</t>
+          <t>Age units - typically 'YEARS' for adult studies</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DTHFL</t>
+          <t>RFSTDTC</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Subject Death Flag</t>
+          <t>Subject Reference Start Date/Time</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1154,7 +1174,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Perm</t>
+          <t>Req</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1165,29 +1185,25 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>DERIVE</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>NY (Y=Yes, N=No)</t>
-        </is>
-      </c>
+          <t>DATE_FORMAT</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Expected variable - death flag, set to Y if subject died during study</t>
+          <t>Subject reference start date - typically informed consent date or first study procedure. Requires integration with other domains</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AGE</t>
+          <t>RFENDTC</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Subject Reference End Date/Time</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1197,40 +1213,36 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Req</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>DOB</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Calculate age using DOB and RFSTDTC</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>DERIVE</t>
+          <t>DATE_FORMAT</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Calculate age in years from DOB (format: YYYYMMDD) to reference start date, requires RFSTDTC</t>
+          <t>Subject reference end date - last known contact or study participation end. Requires integration with disposition/completion data</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AGEU</t>
+          <t>RFXSTDTC</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Age Units</t>
+          <t>Date/Time of First Study Treatment</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1240,7 +1252,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1254,26 +1266,22 @@
           <t>DERIVE</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>AGEU (YEARS, MONTHS, WEEKS, DAYS)</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Age units - set to 'YEARS' as standard for adult studies</t>
+          <t>Date/time of first study treatment. Derived from EX domain EXSTDTC (start date of first exposure)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RACE</t>
+          <t>RFXENDTC</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>Date/Time of Last Study Treatment</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1283,44 +1291,36 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>RCE</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Map source race values to CDISC RACE codelist</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>MAP</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>RACE (WHITE, BLACK OR AFRICAN AMERICAN, ASIAN, AMERICAN INDIAN OR ALASKA NATIVE, NATIVE HAWAIIAN OR OTHER PACIFIC ISLANDER, MULTIPLE, OTHER, UNKNOWN)</t>
-        </is>
-      </c>
+          <t>DERIVE</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Map source RCE to CDISC race codelist. Note: HISPANIC is typically ethnicity not race - may need data clarification</t>
+          <t>Date/time of last study treatment. Derived from EX domain EXENDTC (end date of last exposure)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ETHNIC</t>
+          <t>RFICDTC</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>Date/Time of Informed Consent</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1330,49 +1330,41 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>RCE</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Map HISPANIC values from RCE to ethnicity, others to NOT HISPANIC OR LATINO</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>MAP</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>ETHNIC (HISPANIC OR LATINO, NOT HISPANIC OR LATINO, NOT REPORTED, UNKNOWN)</t>
-        </is>
-      </c>
+          <t>DATE_FORMAT</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Expected variable - derive ethnicity, particularly if RCE contains HISPANIC which is ethnicity not race</t>
+          <t>Date/time of informed consent - typically from separate informed consent form data</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ACTARMCD</t>
+          <t>RFPENDTC</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Actual Arm Code</t>
+          <t>Date/Time of End of Participation</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1388,25 +1380,25 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>DERIVE</t>
+          <t>DATE_FORMAT</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Expected variable - actual arm code, derive from treatment exposure or disposition data</t>
+          <t>Date/time of end of participation - from disposition records or last contact</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ACTARM</t>
+          <t>DTHDTC</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Description of Actual Arm</t>
+          <t>Date/Time of Death</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1427,25 +1419,25 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>DERIVE</t>
+          <t>DATE_FORMAT</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Expected variable - description of actual arm, derive from treatment exposure or disposition data</t>
+          <t>Date/time of death - only populate if subject died during study. Source from death report or AE domain</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>INVID</t>
+          <t>DTHFL</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Investigator Identifier</t>
+          <t>Subject Death Flag</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1460,35 +1452,35 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>INVSITE</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Extract investigator identifier from INVSITE</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
           <t>DERIVE</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Permissible variable - investigator identifier extracted from INVSITE (component after underscore)</t>
+          <t>Subject death flag - 'Y' if subject died, otherwise typically left null or 'N'</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>INVNAM</t>
+          <t>INVID</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Investigator Name</t>
+          <t>Investigator Identifier</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1503,10 +1495,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
+          <t>INVSITE</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Extract investigator ID from INVSITE</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr">
         <is>
           <t>DERIVE</t>
@@ -1515,19 +1511,19 @@
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Permissible variable - investigator name, needs to be sourced from site/investigator reference data</t>
+          <t>Investigator identifier - extracted from second part of INVSITE after underscore</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BRTHDTC</t>
+          <t>INVNAM</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Date/Time of Birth</t>
+          <t>Investigator Name</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1537,19 +1533,15 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>DOB</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Convert DOB from YYYYMMDD integer to ISO 8601 format YYYY-MM-DD</t>
-        </is>
-      </c>
+          <t>[derived]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>DERIVE</t>
@@ -1558,24 +1550,24 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Permissible variable - convert date of birth from integer format to ISO 8601 string format</t>
+          <t>Investigator name - requires reference data linking investigator ID to name</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DMDTC</t>
+          <t>DMSEQ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Date/Time of Collection</t>
+          <t>DMSEQ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t>Num</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1591,30 +1583,30 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>DATE_FORMAT</t>
+          <t>DERIVE</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Permissible variable - date/time of demographics data collection, typically baseline visit date</t>
+          <t>Sequence number for DM domain - always 1 since there is only one record per subject in DM</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DMDY</t>
+          <t>DMDTC</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Study Day of Collection</t>
+          <t>Date/Time of Collection</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1624,31 +1616,35 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[derived]</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
+          <t>DOB</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Use collection date from demographics form</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>DERIVE</t>
+          <t>DATE_FORMAT</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Permissible variable - study day of demographics collection relative to RFSTDTC</t>
+          <t>Date/time of demographics collection - typically the baseline visit date</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DMSEQ</t>
+          <t>DMDY</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DMSEQ</t>
+          <t>Study Day of Collection</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1675,7 +1671,7 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Sequence number for DM domain - always 1 as there is one record per subject</t>
+          <t>Study day of demographics collection relative to RFSTDTC. Positive for dates on/after RFSTDTC, negative before</t>
         </is>
       </c>
     </row>
@@ -1778,7 +1774,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-27T16:40:16.487498</t>
+          <t>2026-01-30T17:08:43.482711</t>
         </is>
       </c>
     </row>
@@ -1893,7 +1889,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Parse PT='01-01' to extract '01' as SUBJID (characters after hyphen)</t>
+          <t>Extract characters after hyphen from PT (e.g., '01' from '01-01')</t>
         </is>
       </c>
     </row>
@@ -1905,31 +1901,31 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Parse PT='01-01' to extract '01' as SITEID (characters before hyphen)</t>
+          <t>Extract characters before hyphen from PT (e.g., '01' from '01-01')</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ARMCD</t>
+          <t>RACE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>To be derived from randomization or treatment assignment data (not available in demographics source)</t>
+          <t>Map RCE: 'BLACK' -&gt; 'BLACK OR AFRICAN AMERICAN', 'ASIAN' -&gt; 'ASIAN', 'HISPANIC' -&gt; 'OTHER' (Hispanic is ethnicity not race)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ARM</t>
+          <t>ETHNIC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>To be derived from randomization or treatment assignment data (not available in demographics source)</t>
+          <t>If RCE='HISPANIC' then 'HISPANIC OR LATINO', else 'NOT HISPANIC OR LATINO'</t>
         </is>
       </c>
     </row>
@@ -1941,223 +1937,223 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Parse INVSITE='C008_408' where 'C008' likely represents country code, map to ISO 3166-1 alpha-3 format</t>
+          <t>Parse INVSITE 'C008_408' where C008 represents country. Map to ISO 3166-1 alpha-3 country code</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RFSTDTC</t>
+          <t>ARMCD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>To be derived from first study activity date (typically from exposure or visit domains)</t>
+          <t>Lookup from randomization/treatment assignment data (not available in demographics source)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RFENDTC</t>
+          <t>ARM</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>To be derived from last study activity date (typically from disposition or visit domains)</t>
+          <t>Lookup from randomization/treatment assignment data (not available in demographics source)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RFXSTDTC</t>
+          <t>ACTARMCD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>To be derived from exposure domain - date of first study treatment</t>
+          <t>Lookup from actual treatment received (EX domain or disposition data)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RFXENDTC</t>
+          <t>ACTARM</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>To be derived from exposure domain - date of last study treatment</t>
+          <t>Lookup from actual treatment received (EX domain or disposition data)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RFICDTC</t>
+          <t>BRTHDTC</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>To be derived from informed consent date in enrollment/disposition data</t>
+          <t>Convert DOB from format 19740918 to '1974-09-18'</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>RFPENDTC</t>
+          <t>RFSTDTC</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>To be derived from disposition domain - date of end of participation</t>
+          <t>Minimum date from: informed consent date, first visit date, randomization date, or first treatment date across all domains</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DTHDTC</t>
+          <t>RFENDTC</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>To be derived from disposition or adverse events if death occurred, otherwise null</t>
+          <t>Maximum date from: last visit date, study completion date, early termination date, or death date across all domains</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DTHFL</t>
+          <t>RFXSTDTC</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Set to 'Y' if DTHDTC is not null, otherwise null</t>
+          <t>Minimum EXSTDTC from EX domain for the subject</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RACE</t>
+          <t>RFXENDTC</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Map RCE values: 'BLACK' -&gt; 'BLACK OR AFRICAN AMERICAN', 'ASIAN' -&gt; 'ASIAN', 'HISPANIC' -&gt; Check if ethnicity or race context</t>
+          <t>Maximum EXENDTC from EX domain for the subject</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ETHNIC</t>
+          <t>RFICDTC</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>If RCE='HISPANIC' then 'HISPANIC OR LATINO', else 'NOT HISPANIC OR LATINO' or null if unknown</t>
+          <t>Informed consent date from ICF or screening module, converted to ISO 8601 format</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ACTARMCD</t>
+          <t>RFPENDTC</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>To be derived from actual treatment received (may differ from planned ARM)</t>
+          <t>Study participation end date from disposition (DS domain) or last study contact</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ACTARM</t>
+          <t>DTHDTC</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>To be derived from actual treatment received (may differ from planned ARM)</t>
+          <t>Death date from adverse events (AE domain), disposition (DS domain), or death form if DTHFL='Y'</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>INVID</t>
+          <t>DTHFL</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Parse INVSITE='C008_408' to extract '_408' as investigator ID</t>
+          <t>If DTHDTC is populated then 'Y', else null or 'N' based on sponsor preference</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>INVNAM</t>
+          <t>INVID</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>To be sourced from investigator master data or site information</t>
+          <t>Extract investigator identifier from INVSITE field (e.g., '408' from 'C008_408')</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BRTHDTC</t>
+          <t>INVNAM</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Transform DOB=19740918 to '1974-09-18' format</t>
+          <t>Look up investigator name based on INVID from site/investigator reference data</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DMDTC</t>
+          <t>DMSEQ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Typically same as visit date for BASELINE visit, needs to be sourced from visit data</t>
+          <t>Sequence number = 1 for DM domain (one record per subject)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DMDY</t>
+          <t>DMDTC</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Calculate study day: DMDTC - RFSTDTC + 1 if DMDTC &gt;= RFSTDTC, else DMDTC - RFSTDTC</t>
+          <t>Date of demographics data collection - can use visit date or baseline date associated with CPEVENT='BASELINE'</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DMSEQ</t>
+          <t>DMDY</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Set to 1 for single demographics record per subject</t>
+          <t>If DMDTC &gt;= RFSTDTC then (DMDTC - RFSTDTC) + 1, else (DMDTC - RFSTDTC)</t>
         </is>
       </c>
     </row>

</xml_diff>